<commit_message>
Update calc and gpu sheet
</commit_message>
<xml_diff>
--- a/benchmark/gpu.xlsx
+++ b/benchmark/gpu.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qx56j\Downloads\mlcm-tomo\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ED81958E-F652-4F26-9B16-F96BC96C6691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF95884-C7F9-4023-9D40-1D56DA2D0B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -32,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,7 +525,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2841,7 +2854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView topLeftCell="A68" workbookViewId="0">
@@ -3949,14 +3962,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">

</xml_diff>